<commit_message>
LINQ queries and documentation
- LINQ queries : Code, SQL optimizations.
- LINQ queries documenation : texts reordered.
</commit_message>
<xml_diff>
--- a/Moureu_Stephane_4_Documentation_de_la_base_de_données_052024_v1.1.xlsx
+++ b/Moureu_Stephane_4_Documentation_de_la_base_de_données_052024_v1.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smour\Documents\@@Privé\@xfiles - copy PC\Documents\@Pro\@Formation\20231018_CPF dev app backend .NET\Projet\Projet 06\Livrables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F97C087-C35A-4448-8311-2A2FBCBC4E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459B16CF-403A-414B-99D7-45CE8A3E3C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="-14205" windowWidth="28305" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3585" windowWidth="27165" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -75,719 +75,10 @@
     <t>Statut Incident, Produit, Version, mots-clé 1, 2 et 3.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : en cours  // Produit : null // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null =&gt; 6 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-06_Incidents en cours_Mot-clé-1 utilisateurs.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : en cours  // Produit : Planificateur d'Anxiété Sociale // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : application // Mot-clé 3 : accessibilité =&gt; 2 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-07_Incidents en cours_Planificateur d'Anxiété Sociale_Mot-clé-1 utilisateurs_Mot-clé-2 application_Mot-clé-3 d'accessibilité.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : en cours  // Produit : Planificateur d'Anxiété Sociale // Version : 1.0 // Mot-clé 1 : utilisateurs // Mot-clé 2 : application // Mot-clé 3 : accessibilité =&gt; 2 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-08_Incidents en cours_Planificateur d'Anxiété Sociale_1.0_Mot-clé-1 utilisateurs_Mot-clé-2 application_Mot-clé-3 accessibilité.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>16</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : résolu // Produit : null // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null =&gt; 13  tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-16_Incidents résolus_Mot-clé-1 utilisateurs.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>17</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : résolu  // Produit : Trader en Herbe // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null =&gt; 2 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-17_Incidents résolus_trader en Herbe_Mot-clé-1 utilisateurs.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>18</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : résolu  // Produit : Trader en Herbe // Version : 1.2 // Mot-clé 1 : utilisateurs // Mot-clé 2 : application // Mot-clé 3 : accessibilité =&gt; 2 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-18_Incidents résolus_trader en Herbe_1.2_Mot-clé-1 utilisateurs.xlsx.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">Par requête NexaWorks </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: conditions de test =&gt; résultat attendu ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>fichier excel des résultats.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : en cours // Produit : null // Version : null =&gt; 8 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-01_Incidents en cours.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">:  Incidents : en cours // Produit : Planificateur d'Entraînement // Version : null =&gt;  2 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">Req-02_Incidents en cours_Planificateur d'Entrainement.xlsx.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>: Incidents : en cours // Produit : Planificateur d'Anxiété Sociale // Version : 1.1 =&gt; 2 tickets</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-03_Incidents en cours_Planificateur d'Anxiété Sociale_1.1.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>: Incidents : résolu // Produit : null // Version : null =&gt; 17 tickets  ==&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> Req-04_Incidents résolus.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incident : résolu // Produit : Planificateur d'Entraînement // Version : null =&gt; 5 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-05_Incidents résolus_Planificateur d'Entraînement.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>13</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incident : résolu // Produit Planificateur d'Entraînement // Version 2.0 =&gt; 2 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-06_Incidents résolus_Planificateur d'Entraînement_2.0.xlsx.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : en cours  et résolus // Produit : Trader en Herbe // Version : null // Début période : 2023-02-01 // Fin période : 2023-02-28 =&gt;  3 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-04_Incidents en cours et résolus_Trader en Herbe_Du 2023-02-01 au 2023-02-28.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>: Incidents : en cours  et résolus // Produit : Maître des Investissements // Version : 2.1 // Début période : 2023-02-01 // Fin période : 2023-02-28 =&gt; 3 tickets ==&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> Req-05_Incidents en cours et résolus_Maître des Investissements_2.1_Du 2023-02-01 au 2023-02-28.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>14</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>: Incidents : résolus // Produit : Trader en Herbe // Version : null // Début période : 2023-02-01 // Fin période : 2023-02-28 =&gt; 2 tickets ==&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> Req-14_Incidents résolus_Trader en Herbe_Du 2023-02-01 au 2023-02-28.xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : résolus // Produit : Maître des Investissements // Version : 2.1 // Début période : 2023-02-01 // Fin période : 2023-02-28 =&gt; 2 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-15_Incidents résolus_Maître des Investissements_2.1_Du 2023-02-01 au 2023-02-28.xlsx.</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Statut Incident, Produit, Version, dates début et fin de période. </t>
   </si>
   <si>
     <t>Statut Incident, Produit, Version, mots-clé 1, 2 et 3, dates début et fin de période.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>: Incidents : en cours  et résolus // Produit : Planificateur d'Anxiété Sociale  // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : application // Mot-clé 3 : null // Début période : 2023-02-01 // Fin période : 2023-06-30  =&gt; 3 tickets ==&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> Req-09_Incidents en cours et résolus_Planificateur d'Anxiété Sociale_Mot-clé-1 utilisateurs_Mot-clé-2 application_Du 2023-02-01 au 2023-06-30..xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : en cours  et résolus // Produit : Planificateur d'Anxiété Sociale  // Version : 1.1 // Mot-clé 1 : utilisateurs // Mot-clé 2 : application // Mot-clé 3 : null // Début période : 2023-02-01 // Fin période : 2023-06-30  =&gt; 2 tickets ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-10_Incidents en cours et résolus_Planificateur d'Anxiété Sociale_1.1_Mot-clé-1 utilisateurs_Mot-clé-2 application_Du 2023-02-01 au 2023-06-30..xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>19</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>: Incidents : résolus // Produit :Trader en Herbe  // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null // Début période : 2023-02-01 // Fin période : 2023-06-30 =&gt; 3 tickets ==&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> Req-19_Incidents résolus_Trader en Herbe_Mot-clé-1 utilisateurs_Du 2023-02-01 au 2023-06-30..xlsx.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">: Incidents : résolus // Produit :Trader en Herbe  // Version : 1.1 // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null // Début période : 2023-02-01 // Fin période : 2023-06-30 =&gt; 1 ticket ==&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>Req-20_Incidents résolus_Trader en Herbe_1.1_Mot-clé-1 utilisateurs_Du 2023-02-01 au 2023-06-30..xlsx.</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Obtenir les problèmes en cours ou résolus contenant une liste de mots-clés pour tous les produits, ou pour un produit et toutes ses versions, ou pour un produit et une version.
@@ -823,6 +114,1083 @@
         <rFont val="Montserrat"/>
       </rPr>
       <t>OK</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">Par requête NexaWorks </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: conditions de test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">=&gt; résultat attendu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>fichier excel des résultats.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : en cours  et résolus // Produit : Planificateur d'Anxiété Sociale  // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : application // Mot-clé 3 : null // Début période : 2023-02-01 // Fin période : 2023-06-30  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">=&gt; 3 tickets 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>==&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> Req-09_Incidents en cours et résolus_Planificateur d'Anxiété Sociale_Mot-clé-1 utilisateurs_Mot-clé-2 application_Du 2023-02-01 au 2023-06-30..xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : en cours  et résolus // Produit : Planificateur d'Anxiété Sociale  // Version : 1.1 // Mot-clé 1 : utilisateurs // Mot-clé 2 : application // Mot-clé 3 : null // Début période : 2023-02-01 // Fin période : 2023-06-30  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">=&gt; 2 tickets 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-10_Incidents en cours et résolus_Planificateur d'Anxiété Sociale_1.1_Mot-clé-1 utilisateurs_Mot-clé-2 application_Du 2023-02-01 au 2023-06-30..xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>: Incidents : résolus // Produit :Trader en Herbe  // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null // Début période : 2023-02-01 // Fin période : 2023-06-30</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> =&gt; 3 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+ ==&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> Req-19_Incidents résolus_Trader en Herbe_Mot-clé-1 utilisateurs_Du 2023-02-01 au 2023-06-30..xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : résolus // Produit :Trader en Herbe  // Version : 1.1 // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null // Début période : 2023-02-01 // Fin période : 2023-06-30 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 1 ticket</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+ ==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-20_Incidents résolus_Trader en Herbe_1.1_Mot-clé-1 utilisateurs_Du 2023-02-01 au 2023-06-30..xlsx.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : en cours  et résolus // Produit : Trader en Herbe // Version : null // Début période : 2023-02-01 // Fin période : 2023-02-28 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt;  3 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> 
+==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-04_Incidents en cours et résolus_Trader en Herbe_Du 2023-02-01 au 2023-02-28.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : en cours  et résolus // Produit : Maître des Investissements // Version : 2.1 // Début période : 2023-02-01 // Fin période : 2023-02-28 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 3 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> 
+==&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> Req-05_Incidents en cours et résolus_Maître des Investissements_2.1_Du 2023-02-01 au 2023-02-28.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : résolus // Produit : Trader en Herbe // Version : null // Début période : 2023-02-01 // Fin période : 2023-02-28 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 2 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> 
+==&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> Req-14_Incidents résolus_Trader en Herbe_Du 2023-02-01 au 2023-02-28.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : résolus // Produit : Maître des Investissements // Version : 2.1 // Début période : 2023-02-01 // Fin période : 2023-02-28 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">=&gt; 2 tickets
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> ==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-15_Incidents résolus_Maître des Investissements_2.1_Du 2023-02-01 au 2023-02-28.xlsx.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : en cours // Produit : null // Version : null </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 8 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> 
+==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-01_Incidents en cours.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">:  Incidents : en cours // Produit : Planificateur d'Entraînement // Version : null </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">=&gt;  2 tickets 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">Req-02_Incidents en cours_Planificateur d'Entrainement.xlsx.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : en cours // Produit : Planificateur d'Anxiété Sociale // Version : 1.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 2 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-03_Incidents en cours_Planificateur d'Anxiété Sociale_1.1.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : résolu // Produit : null // Version : null </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 17 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">  
+==&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> Req-04_Incidents résolus.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incident : résolu // Produit : Planificateur d'Entraînement // Version : null </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">=&gt; 5 tickets 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-05_Incidents résolus_Planificateur d'Entraînement.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incident : résolu // Produit Planificateur d'Entraînement // Version 2.0 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 2 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> 
+==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-06_Incidents résolus_Planificateur d'Entraînement_2.0.xlsx.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : en cours  // Produit : null // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 6 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> 
+==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-06_Incidents en cours_Mot-clé-1 utilisateurs.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : en cours  // Produit : Planificateur d'Anxiété Sociale // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : application // Mot-clé 3 : accessibilité </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 2 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> 
+==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-07_Incidents en cours_Planificateur d'Anxiété Sociale_Mot-clé-1 utilisateurs_Mot-clé-2 application_Mot-clé-3 d'accessibilité.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : en cours  // Produit : Planificateur d'Anxiété Sociale // Version : 1.0 // Mot-clé 1 : utilisateurs // Mot-clé 2 : application // Mot-clé 3 : accessibilité </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 1 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> 
+==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-08_Incidents en cours_Planificateur d'Anxiété Sociale_1.0_Mot-clé-1 utilisateurs_Mot-clé-2 application_Mot-clé-3 accessibilité.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : résolu // Produit : null // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 13  tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> 
+==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-16_Incidents résolus_Mot-clé-1 utilisateurs.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : résolu  // Produit : Trader en Herbe // Version : nulll // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>=&gt; 4 tickets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> ==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-17_Incidents résolus_trader en Herbe_Mot-clé-1 utilisateurs.xlsx.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">: Incidents : résolu  // Produit : Trader en Herbe // Version : 1.2 // Mot-clé 1 : utilisateurs // Mot-clé 2 : null // Mot-clé 3 : null  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">=&gt; 2 tickets 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">==&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>Req-18_Incidents résolus_trader en Herbe_1.2_Mot-clé-1 utilisateurs.xlsx.</t>
     </r>
   </si>
 </sst>
@@ -1146,13 +1514,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1184,6 +1545,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1429,29 +1797,27 @@
   </sheetPr>
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="87.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="55" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="102.140625" customWidth="1"/>
+    <col min="6" max="6" width="121.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1464,13 +1830,13 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1526,15 +1892,15 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="19" t="s">
-        <v>18</v>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="14" t="s">
+        <v>25</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1546,24 +1912,24 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="154.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:15" ht="193.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>29</v>
+      <c r="E6" s="10" t="s">
+        <v>24</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>19</v>
+      <c r="F6" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1575,24 +1941,24 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="172.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:15" ht="189" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>26</v>
+      <c r="E7" s="10" t="s">
+        <v>24</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>20</v>
+      <c r="F7" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1604,24 +1970,24 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="236.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+    <row r="8" spans="1:15" ht="267" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>28</v>
+      <c r="B8" s="10" t="s">
+        <v>23</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>17</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1633,24 +1999,24 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="214.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+    <row r="9" spans="1:15" ht="222.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>25</v>
+      <c r="C9" s="10" t="s">
+        <v>18</v>
       </c>
-      <c r="E9" s="15" t="s">
-        <v>29</v>
+      <c r="D9" s="10" t="s">
+        <v>20</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>23</v>
+      <c r="E9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1663,12 +2029,12 @@
       <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="18"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1680,12 +2046,12 @@
       <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="24"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1697,12 +2063,12 @@
       <c r="O11" s="1"/>
     </row>
     <row r="12" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="24"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1714,12 +2080,12 @@
       <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="24"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1731,12 +2097,12 @@
       <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="24"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>

</xml_diff>